<commit_message>
Close antonyko-hwte/new_sw#3 요구사항 명세서
</commit_message>
<xml_diff>
--- a/docs/요구사항 명세서.xlsx
+++ b/docs/요구사항 명세서.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Personal Info\06.SNS_카페_블로그 등\01.블로그\프로젝트관리 산출물\SI 프로젝트\06 산출물\02 분석단계\요구사항정의서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB12469F-78DB-4586-988C-32761631CF7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7185BD98-1C1A-488B-BE05-2D79187FECBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="170" yWindow="0" windowWidth="17800" windowHeight="9970" xr2:uid="{805F09F1-BD61-458A-A67B-FDCA23435B12}"/>
+    <workbookView xWindow="30705" yWindow="1905" windowWidth="23940" windowHeight="13485" xr2:uid="{805F09F1-BD61-458A-A67B-FDCA23435B12}"/>
   </bookViews>
   <sheets>
     <sheet name="요구사항정의서" sheetId="1" r:id="rId1"/>
@@ -228,11 +228,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>요구사항 정의서 (Requirment Definition)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Template by 쓰루(https://blog.naver.com/sunhoskm, email:sunhoskm@naver.com)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">요구사항 정의서 (Requirment Definition) </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -457,7 +457,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -581,15 +581,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -605,9 +602,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -645,7 +642,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -751,7 +748,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -893,7 +890,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -907,12 +904,12 @@
       <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.4140625" style="13" customWidth="1"/>
+    <col min="1" max="2" width="11.375" style="13" customWidth="1"/>
     <col min="3" max="3" width="10" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.75" style="14" customWidth="1"/>
@@ -920,31 +917,31 @@
     <col min="7" max="8" width="10" style="14" customWidth="1"/>
     <col min="9" max="9" width="17.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="24" style="1" customWidth="1"/>
-    <col min="11" max="12" width="12.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.9140625" style="1" customWidth="1"/>
-    <col min="14" max="16" width="16.1640625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.6640625" style="1"/>
+    <col min="11" max="12" width="12.375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.875" style="1" customWidth="1"/>
+    <col min="14" max="16" width="16.125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="15"/>
-    </row>
-    <row r="2" spans="1:16" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="35" t="s">
-        <v>42</v>
-      </c>
       <c r="B2" s="15"/>
     </row>
-    <row r="3" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="34"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
@@ -958,7 +955,7 @@
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
     </row>
-    <row r="4" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>39</v>
       </c>
@@ -978,7 +975,7 @@
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
     </row>
-    <row r="5" spans="1:16" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="16"/>
@@ -995,8 +992,8 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:16" ht="9" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="7" spans="1:16" ht="48" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:16" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>8</v>
       </c>
@@ -1046,7 +1043,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="58" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" ht="48" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>20</v>
       </c>
@@ -1088,7 +1085,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="32" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A9" s="28"/>
       <c r="B9" s="27" t="s">
         <v>26</v>
@@ -1118,7 +1115,7 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
     </row>
-    <row r="10" spans="1:16" ht="32" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A10" s="28"/>
       <c r="B10" s="28"/>
       <c r="C10" s="12" t="s">
@@ -1146,7 +1143,7 @@
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
     </row>
-    <row r="11" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="C11" s="32" t="s">
@@ -1174,7 +1171,7 @@
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
     </row>
-    <row r="12" spans="1:16" ht="32" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" ht="27" x14ac:dyDescent="0.3">
       <c r="A12" s="28"/>
       <c r="B12" s="28"/>
       <c r="C12" s="12" t="s">
@@ -1200,7 +1197,7 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="29"/>
       <c r="B13" s="31"/>
       <c r="C13" s="4"/>
@@ -1218,7 +1215,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1236,7 +1233,7 @@
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1254,7 +1251,7 @@
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1272,7 +1269,7 @@
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1290,7 +1287,7 @@
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1308,7 +1305,7 @@
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1326,7 +1323,7 @@
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1344,7 +1341,7 @@
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1362,7 +1359,7 @@
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1380,7 +1377,7 @@
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1398,7 +1395,7 @@
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1416,7 +1413,7 @@
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1434,7 +1431,7 @@
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1452,7 +1449,7 @@
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -1470,7 +1467,7 @@
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1488,7 +1485,7 @@
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -1506,7 +1503,7 @@
       <c r="O29" s="8"/>
       <c r="P29" s="8"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -1524,7 +1521,7 @@
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1542,7 +1539,7 @@
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -1560,7 +1557,7 @@
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -1578,7 +1575,7 @@
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -1596,7 +1593,7 @@
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -1614,7 +1611,7 @@
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1632,7 +1629,7 @@
       <c r="O36" s="8"/>
       <c r="P36" s="8"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -1650,7 +1647,7 @@
       <c r="O37" s="8"/>
       <c r="P37" s="8"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -1668,7 +1665,7 @@
       <c r="O38" s="8"/>
       <c r="P38" s="8"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -1686,7 +1683,7 @@
       <c r="O39" s="8"/>
       <c r="P39" s="8"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -1704,7 +1701,7 @@
       <c r="O40" s="8"/>
       <c r="P40" s="8"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -1722,7 +1719,7 @@
       <c r="O41" s="8"/>
       <c r="P41" s="8"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>

</xml_diff>

<commit_message>
Close antonyko-hwte/new_system#3 요구사항 명세서
</commit_message>
<xml_diff>
--- a/docs/요구사항 명세서.xlsx
+++ b/docs/요구사항 명세서.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7185BD98-1C1A-488B-BE05-2D79187FECBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0D8755-E58E-4FD5-AB1A-EB950E2D14CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30705" yWindow="1905" windowWidth="23940" windowHeight="13485" xr2:uid="{805F09F1-BD61-458A-A67B-FDCA23435B12}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">요구사항 정의서 (Requirment Definition) </t>
+    <t>요구사항 정의서 (Requirment Definition)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>